<commit_message>
Corregir codigo escobaBall, prim y escaleras
</commit_message>
<xml_diff>
--- a/BorgesCano.Adrian_GonzalezMartinez.Marco_PL4/Problema6Tema4.xlsx
+++ b/BorgesCano.Adrian_GonzalezMartinez.Marco_PL4/Problema6Tema4.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CosasUni\AYC\LABAYC\BorgesCano.Adrian_GonzalezMartinez.Marco_PL4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DBF773E-2FBE-4BE8-AF75-B0140F0DB784}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954F4EEA-6CD6-4810-A008-EB2074BD2D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1CE05A40-D737-4540-8C11-EE9F2B100FB5}"/>
   </bookViews>
@@ -540,6 +540,42 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -566,42 +602,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -925,7 +925,7 @@
   <dimension ref="B1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L20" sqref="L20"/>
+      <selection activeCell="J12" sqref="J12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -937,81 +937,81 @@
     <row r="2" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="5"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="10" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="10"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="10"/>
-      <c r="H2" s="10"/>
-      <c r="I2" s="10"/>
-      <c r="J2" s="10"/>
-      <c r="K2" s="10"/>
-      <c r="L2" s="10"/>
-      <c r="M2" s="10"/>
-      <c r="N2" s="10"/>
-      <c r="O2" s="10"/>
-      <c r="P2" s="10"/>
-      <c r="Q2" s="10"/>
-      <c r="R2" s="11"/>
+      <c r="D2" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="22"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="23"/>
     </row>
     <row r="3" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="19">
-        <v>0</v>
-      </c>
-      <c r="E3" s="20"/>
-      <c r="F3" s="20"/>
-      <c r="G3" s="20"/>
-      <c r="H3" s="21"/>
-      <c r="I3" s="19">
-        <v>1</v>
-      </c>
-      <c r="J3" s="20"/>
-      <c r="K3" s="20"/>
-      <c r="L3" s="20"/>
-      <c r="M3" s="21"/>
-      <c r="N3" s="19">
-        <v>2</v>
-      </c>
-      <c r="O3" s="20"/>
-      <c r="P3" s="20"/>
-      <c r="Q3" s="20"/>
-      <c r="R3" s="21"/>
+      <c r="D3" s="17">
+        <v>0</v>
+      </c>
+      <c r="E3" s="18"/>
+      <c r="F3" s="18"/>
+      <c r="G3" s="18"/>
+      <c r="H3" s="19"/>
+      <c r="I3" s="17">
+        <v>1</v>
+      </c>
+      <c r="J3" s="18"/>
+      <c r="K3" s="18"/>
+      <c r="L3" s="18"/>
+      <c r="M3" s="19"/>
+      <c r="N3" s="17">
+        <v>2</v>
+      </c>
+      <c r="O3" s="18"/>
+      <c r="P3" s="18"/>
+      <c r="Q3" s="18"/>
+      <c r="R3" s="19"/>
     </row>
     <row r="4" spans="2:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="14">
+      <c r="B4" s="20" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="26">
         <v>0</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="17"/>
-      <c r="H4" s="18"/>
+      <c r="F4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="15"/>
+      <c r="H4" s="16"/>
       <c r="I4" s="5"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="17"/>
-      <c r="M4" s="18"/>
+      <c r="K4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="15"/>
+      <c r="M4" s="16"/>
       <c r="N4" s="5"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="17"/>
-      <c r="R4" s="18"/>
+      <c r="P4" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="15"/>
+      <c r="R4" s="16"/>
     </row>
     <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="8"/>
-      <c r="C5" s="15"/>
+      <c r="B5" s="20"/>
+      <c r="C5" s="27"/>
       <c r="D5" s="6"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1">
@@ -1047,170 +1047,170 @@
       </c>
     </row>
     <row r="6" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="8"/>
-      <c r="C6" s="15"/>
-      <c r="D6" s="12" t="s">
+      <c r="B6" s="20"/>
+      <c r="C6" s="27"/>
+      <c r="D6" s="24" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="1">
         <v>0</v>
       </c>
-      <c r="F6" s="22">
-        <v>1</v>
-      </c>
-      <c r="G6" s="22" t="s">
+      <c r="F6" s="8">
+        <v>1</v>
+      </c>
+      <c r="G6" s="8" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="23" t="s">
+      <c r="H6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="12" t="s">
+      <c r="I6" s="24" t="s">
         <v>3</v>
       </c>
       <c r="J6" s="1">
         <v>0</v>
       </c>
-      <c r="K6" s="22" t="s">
+      <c r="K6" s="8" t="s">
         <v>6</v>
       </c>
-      <c r="L6" s="22" t="s">
+      <c r="L6" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="M6" s="23" t="s">
+      <c r="M6" s="9" t="s">
         <v>13</v>
       </c>
-      <c r="N6" s="12" t="s">
+      <c r="N6" s="24" t="s">
         <v>3</v>
       </c>
       <c r="O6" s="1">
         <v>0</v>
       </c>
-      <c r="P6" s="26" t="s">
+      <c r="P6" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="Q6" s="26" t="s">
+      <c r="Q6" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="R6" s="23">
+      <c r="R6" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="8"/>
-      <c r="C7" s="15"/>
-      <c r="D7" s="12"/>
+      <c r="B7" s="20"/>
+      <c r="C7" s="27"/>
+      <c r="D7" s="24"/>
       <c r="E7" s="1">
         <v>1</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="8" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="8" t="s">
         <v>15</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="I7" s="12"/>
+      <c r="I7" s="24"/>
       <c r="J7" s="1">
         <v>1</v>
       </c>
-      <c r="K7" s="22" t="s">
+      <c r="K7" s="8" t="s">
         <v>17</v>
       </c>
-      <c r="L7" s="22" t="s">
+      <c r="L7" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="M7" s="23" t="s">
+      <c r="M7" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="N7" s="12"/>
+      <c r="N7" s="24"/>
       <c r="O7" s="1">
         <v>1</v>
       </c>
-      <c r="P7" s="26" t="s">
+      <c r="P7" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="Q7" s="26" t="s">
+      <c r="Q7" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="R7" s="23">
+      <c r="R7" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="8" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="8"/>
-      <c r="C8" s="16"/>
-      <c r="D8" s="13"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="25"/>
       <c r="E8" s="4">
         <v>2</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="F8" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="G8" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="H8" s="25">
-        <v>0</v>
-      </c>
-      <c r="I8" s="13"/>
+      <c r="H8" s="11">
+        <v>0</v>
+      </c>
+      <c r="I8" s="25"/>
       <c r="J8" s="4">
         <v>2</v>
       </c>
-      <c r="K8" s="24" t="s">
+      <c r="K8" s="10" t="s">
         <v>24</v>
       </c>
-      <c r="L8" s="24" t="s">
+      <c r="L8" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="M8" s="27">
-        <v>0</v>
-      </c>
-      <c r="N8" s="13"/>
+      <c r="M8" s="13">
+        <v>0</v>
+      </c>
+      <c r="N8" s="25"/>
       <c r="O8" s="4">
         <v>2</v>
       </c>
-      <c r="P8" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q8" s="24">
-        <v>0</v>
-      </c>
-      <c r="R8" s="25">
+      <c r="P8" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q8" s="10">
+        <v>0</v>
+      </c>
+      <c r="R8" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="2:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="8"/>
-      <c r="C9" s="14">
+      <c r="B9" s="20"/>
+      <c r="C9" s="26">
         <v>1</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="17"/>
-      <c r="H9" s="18"/>
+      <c r="F9" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="15"/>
+      <c r="H9" s="16"/>
       <c r="I9" s="5"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="17"/>
-      <c r="M9" s="18"/>
+      <c r="K9" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="15"/>
+      <c r="M9" s="16"/>
       <c r="N9" s="5"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="17"/>
-      <c r="R9" s="18"/>
+      <c r="P9" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="15"/>
+      <c r="R9" s="16"/>
     </row>
     <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="8"/>
-      <c r="C10" s="15"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="27"/>
       <c r="D10" s="6"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1">
@@ -1246,170 +1246,170 @@
       </c>
     </row>
     <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="8"/>
-      <c r="C11" s="15"/>
-      <c r="D11" s="12" t="s">
+      <c r="B11" s="20"/>
+      <c r="C11" s="27"/>
+      <c r="D11" s="24" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="1">
         <v>0</v>
       </c>
-      <c r="F11" s="22" t="s">
+      <c r="F11" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="G11" s="22" t="s">
+      <c r="G11" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="12" t="s">
+      <c r="I11" s="24" t="s">
         <v>3</v>
       </c>
       <c r="J11" s="1">
         <v>0</v>
       </c>
-      <c r="K11" s="22" t="s">
+      <c r="K11" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="L11" s="22" t="s">
+      <c r="L11" s="8" t="s">
         <v>28</v>
       </c>
-      <c r="M11" s="23" t="s">
+      <c r="M11" s="9" t="s">
         <v>29</v>
       </c>
-      <c r="N11" s="12" t="s">
+      <c r="N11" s="24" t="s">
         <v>3</v>
       </c>
       <c r="O11" s="1">
         <v>0</v>
       </c>
-      <c r="P11" s="26" t="s">
+      <c r="P11" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="Q11" s="26" t="s">
+      <c r="Q11" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="R11" s="23">
+      <c r="R11" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="8"/>
-      <c r="C12" s="15"/>
-      <c r="D12" s="12"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="27"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="1">
         <v>1</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F12" s="8" t="s">
         <v>32</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G12" s="8" t="s">
         <v>35</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="I12" s="12"/>
+      <c r="I12" s="24"/>
       <c r="J12" s="1">
         <v>1</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="K12" s="8" t="s">
         <v>37</v>
       </c>
-      <c r="L12" s="22" t="s">
+      <c r="L12" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="M12" s="23" t="s">
+      <c r="M12" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="N12" s="12"/>
+      <c r="N12" s="24"/>
       <c r="O12" s="1">
         <v>1</v>
       </c>
-      <c r="P12" s="26" t="s">
+      <c r="P12" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="Q12" s="26" t="s">
+      <c r="Q12" s="12" t="s">
         <v>41</v>
       </c>
-      <c r="R12" s="23">
+      <c r="R12" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="8"/>
-      <c r="C13" s="16"/>
-      <c r="D13" s="13"/>
+      <c r="B13" s="20"/>
+      <c r="C13" s="28"/>
+      <c r="D13" s="25"/>
       <c r="E13" s="4">
         <v>2</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="F13" s="10" t="s">
         <v>33</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="G13" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="H13" s="25">
-        <v>0</v>
-      </c>
-      <c r="I13" s="13"/>
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="25"/>
       <c r="J13" s="4">
         <v>2</v>
       </c>
-      <c r="K13" s="24" t="s">
+      <c r="K13" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="L13" s="24" t="s">
+      <c r="L13" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="M13" s="25">
-        <v>0</v>
-      </c>
-      <c r="N13" s="13"/>
+      <c r="M13" s="11">
+        <v>0</v>
+      </c>
+      <c r="N13" s="25"/>
       <c r="O13" s="4">
         <v>2</v>
       </c>
-      <c r="P13" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="24">
-        <v>0</v>
-      </c>
-      <c r="R13" s="25">
+      <c r="P13" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>0</v>
+      </c>
+      <c r="R13" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="14" spans="2:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="8"/>
-      <c r="C14" s="14">
+      <c r="B14" s="20"/>
+      <c r="C14" s="26">
         <v>2</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="17"/>
-      <c r="H14" s="18"/>
+      <c r="F14" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="15"/>
+      <c r="H14" s="16"/>
       <c r="I14" s="5"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="L14" s="17"/>
-      <c r="M14" s="18"/>
+      <c r="K14" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="15"/>
+      <c r="M14" s="16"/>
       <c r="N14" s="5"/>
       <c r="O14" s="2"/>
-      <c r="P14" s="17" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="17"/>
-      <c r="R14" s="18"/>
+      <c r="P14" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="15"/>
+      <c r="R14" s="16"/>
     </row>
     <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B15" s="8"/>
-      <c r="C15" s="15"/>
+      <c r="B15" s="20"/>
+      <c r="C15" s="27"/>
       <c r="D15" s="6"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1">
@@ -1445,153 +1445,143 @@
       </c>
     </row>
     <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B16" s="8"/>
-      <c r="C16" s="15"/>
-      <c r="D16" s="12" t="s">
+      <c r="B16" s="20"/>
+      <c r="C16" s="27"/>
+      <c r="D16" s="24" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="1">
         <v>0</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F16" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G16" s="8" t="s">
         <v>45</v>
       </c>
-      <c r="H16" s="23">
-        <v>0</v>
-      </c>
-      <c r="I16" s="12" t="s">
+      <c r="H16" s="9">
+        <v>0</v>
+      </c>
+      <c r="I16" s="24" t="s">
         <v>3</v>
       </c>
       <c r="J16" s="1">
         <v>0</v>
       </c>
-      <c r="K16" s="22" t="s">
+      <c r="K16" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="L16" s="22" t="s">
+      <c r="L16" s="8" t="s">
         <v>48</v>
       </c>
-      <c r="M16" s="23">
-        <v>0</v>
-      </c>
-      <c r="N16" s="12" t="s">
+      <c r="M16" s="9">
+        <v>0</v>
+      </c>
+      <c r="N16" s="24" t="s">
         <v>3</v>
       </c>
       <c r="O16" s="1">
         <v>0</v>
       </c>
-      <c r="P16" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="22">
-        <v>0</v>
-      </c>
-      <c r="R16" s="23">
+      <c r="P16" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>0</v>
+      </c>
+      <c r="R16" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="17" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B17" s="8"/>
-      <c r="C17" s="15"/>
-      <c r="D17" s="12"/>
+      <c r="B17" s="20"/>
+      <c r="C17" s="27"/>
+      <c r="D17" s="24"/>
       <c r="E17" s="1">
         <v>1</v>
       </c>
-      <c r="F17" s="22" t="s">
+      <c r="F17" s="8" t="s">
         <v>34</v>
       </c>
-      <c r="G17" s="22" t="s">
+      <c r="G17" s="8" t="s">
         <v>46</v>
       </c>
-      <c r="H17" s="23">
-        <v>0</v>
-      </c>
-      <c r="I17" s="12"/>
+      <c r="H17" s="9">
+        <v>0</v>
+      </c>
+      <c r="I17" s="24"/>
       <c r="J17" s="1">
         <v>1</v>
       </c>
-      <c r="K17" s="22" t="s">
+      <c r="K17" s="8" t="s">
         <v>49</v>
       </c>
-      <c r="L17" s="22" t="s">
+      <c r="L17" s="8" t="s">
         <v>50</v>
       </c>
-      <c r="M17" s="23">
-        <v>0</v>
-      </c>
-      <c r="N17" s="12"/>
+      <c r="M17" s="9">
+        <v>0</v>
+      </c>
+      <c r="N17" s="24"/>
       <c r="O17" s="1">
         <v>1</v>
       </c>
-      <c r="P17" s="22">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="22">
-        <v>0</v>
-      </c>
-      <c r="R17" s="23">
+      <c r="P17" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>0</v>
+      </c>
+      <c r="R17" s="9">
         <v>0</v>
       </c>
     </row>
     <row r="18" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="9"/>
-      <c r="C18" s="16"/>
-      <c r="D18" s="13"/>
+      <c r="B18" s="21"/>
+      <c r="C18" s="28"/>
+      <c r="D18" s="25"/>
       <c r="E18" s="4">
         <v>2</v>
       </c>
-      <c r="F18" s="24">
-        <v>0</v>
-      </c>
-      <c r="G18" s="24">
-        <v>0</v>
-      </c>
-      <c r="H18" s="25">
-        <v>0</v>
-      </c>
-      <c r="I18" s="13"/>
+      <c r="F18" s="10">
+        <v>0</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0</v>
+      </c>
+      <c r="H18" s="11">
+        <v>0</v>
+      </c>
+      <c r="I18" s="25"/>
       <c r="J18" s="4">
         <v>2</v>
       </c>
-      <c r="K18" s="24">
-        <v>0</v>
-      </c>
-      <c r="L18" s="24">
-        <v>0</v>
-      </c>
-      <c r="M18" s="28">
-        <v>0</v>
-      </c>
-      <c r="N18" s="13"/>
+      <c r="K18" s="10">
+        <v>0</v>
+      </c>
+      <c r="L18" s="10">
+        <v>0</v>
+      </c>
+      <c r="M18" s="14">
+        <v>0</v>
+      </c>
+      <c r="N18" s="25"/>
       <c r="O18" s="4">
         <v>2</v>
       </c>
-      <c r="P18" s="24">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="24">
-        <v>0</v>
-      </c>
-      <c r="R18" s="25">
+      <c r="P18" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="10">
+        <v>0</v>
+      </c>
+      <c r="R18" s="11">
         <v>0</v>
       </c>
     </row>
     <row r="19" spans="2:18" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="26">
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="F4:H4"/>
     <mergeCell ref="B4:B18"/>
     <mergeCell ref="D2:R2"/>
     <mergeCell ref="D11:D13"/>
@@ -1608,6 +1598,16 @@
     <mergeCell ref="C14:C18"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="K9:M9"/>
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Corregir ejercicio 6 tema 4
</commit_message>
<xml_diff>
--- a/BorgesCano.Adrian_GonzalezMartinez.Marco_PL4/Problema6Tema4.xlsx
+++ b/BorgesCano.Adrian_GonzalezMartinez.Marco_PL4/Problema6Tema4.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CosasUni\AYC\LABAYC\BorgesCano.Adrian_GonzalezMartinez.Marco_PL4\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Escritorio\Escrotorio\AESTUDIAR\UAH\2\ALGORITMIA\LABAYC\BorgesCano.Adrian_GonzalezMartinez.Marco_PL4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{954F4EEA-6CD6-4810-A008-EB2074BD2D60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37DD4467-9133-4C99-B6FF-FC8C20A0F5D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{1CE05A40-D737-4540-8C11-EE9F2B100FB5}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{1CE05A40-D737-4540-8C11-EE9F2B100FB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -73,121 +73,121 @@
     <t>PS2</t>
   </si>
   <si>
-    <t>PG·PC</t>
-  </si>
-  <si>
-    <t>PG·PC2</t>
-  </si>
-  <si>
-    <t>PG2·PC</t>
-  </si>
-  <si>
-    <t>PT·PC</t>
-  </si>
-  <si>
-    <t>PT·PC2</t>
-  </si>
-  <si>
-    <t>PG·PT</t>
-  </si>
-  <si>
-    <t>PG·PT·PC</t>
-  </si>
-  <si>
-    <t>PG·PT·PC2</t>
-  </si>
-  <si>
-    <t>PG2·PT</t>
-  </si>
-  <si>
-    <t>PG2·PT·PC</t>
-  </si>
-  <si>
-    <t>PT2·PC</t>
-  </si>
-  <si>
-    <t>PG·PT2·PC</t>
-  </si>
-  <si>
-    <t>PG·PT2</t>
-  </si>
-  <si>
-    <t>PS·PC</t>
-  </si>
-  <si>
-    <t>PS·PC2</t>
-  </si>
-  <si>
-    <t>PG·PS</t>
-  </si>
-  <si>
-    <t>PG·PS·PC</t>
-  </si>
-  <si>
-    <t>PG·PS·PC2</t>
-  </si>
-  <si>
-    <t>PG2·PS</t>
-  </si>
-  <si>
-    <t>PG2·PS·PC</t>
-  </si>
-  <si>
-    <t>PS·PT</t>
-  </si>
-  <si>
-    <t>PS·PT2</t>
-  </si>
-  <si>
-    <t>PS2·PT</t>
-  </si>
-  <si>
-    <t>PS·PT·PC</t>
-  </si>
-  <si>
-    <t>PS·PT·PC2</t>
-  </si>
-  <si>
-    <t>PG·PS·PT</t>
-  </si>
-  <si>
-    <t>PG·PS·PT·PC</t>
-  </si>
-  <si>
-    <t>PG·PS·PT·PC2</t>
-  </si>
-  <si>
-    <t>PG2·PS·PT</t>
-  </si>
-  <si>
-    <t>PG2·PS·PT·PC</t>
-  </si>
-  <si>
-    <t>PS·PT2·PC</t>
-  </si>
-  <si>
-    <t>PG·PS·PT2</t>
-  </si>
-  <si>
-    <t>PG·PS·PT2·PC</t>
-  </si>
-  <si>
-    <t>PS2·PC</t>
-  </si>
-  <si>
-    <t>PS2·PT·PC</t>
-  </si>
-  <si>
-    <t>PG·PS2</t>
-  </si>
-  <si>
-    <t>PG·PS2·PC</t>
-  </si>
-  <si>
-    <t>PG·PS2·PT</t>
-  </si>
-  <si>
-    <t>PG·PS2·PT·PC</t>
+    <t>2·PT·PC</t>
+  </si>
+  <si>
+    <t>2·PT·PC2</t>
+  </si>
+  <si>
+    <t>2·PT2·PC</t>
+  </si>
+  <si>
+    <t>2·PS·PT</t>
+  </si>
+  <si>
+    <t>2·PS·PT2</t>
+  </si>
+  <si>
+    <t>2·PS2·PT</t>
+  </si>
+  <si>
+    <t>2·PS2·PC</t>
+  </si>
+  <si>
+    <t>2·PG·PT</t>
+  </si>
+  <si>
+    <t>2·PG·PS</t>
+  </si>
+  <si>
+    <t>2·PS·PC</t>
+  </si>
+  <si>
+    <t>6·PS·PT·PC</t>
+  </si>
+  <si>
+    <t>2·PG·PC</t>
+  </si>
+  <si>
+    <t>6·PG·PT·PC</t>
+  </si>
+  <si>
+    <t>6·PG·PS·PC</t>
+  </si>
+  <si>
+    <t>6·PG·PS·PT</t>
+  </si>
+  <si>
+    <t>6·PS·PT2·PC</t>
+  </si>
+  <si>
+    <t>6·PS·PT·PC2</t>
+  </si>
+  <si>
+    <t>6·PS2·PT·PC</t>
+  </si>
+  <si>
+    <t>2·PG2·PT</t>
+  </si>
+  <si>
+    <t>2·PG2·PC</t>
+  </si>
+  <si>
+    <t>6·PG2·PT·PC</t>
+  </si>
+  <si>
+    <t>6·PG·PS·PT2</t>
+  </si>
+  <si>
+    <t>6·PG·PS·PC2</t>
+  </si>
+  <si>
+    <t>24·PG·PS·PT·PC</t>
+  </si>
+  <si>
+    <t>6·PG·PT2·PC</t>
+  </si>
+  <si>
+    <t>2·PS·PC2</t>
+  </si>
+  <si>
+    <t>6·PG·PT·PC2</t>
+  </si>
+  <si>
+    <t>2·PG·PT2</t>
+  </si>
+  <si>
+    <t>2·PG·PC2</t>
+  </si>
+  <si>
+    <t>2·PG2·PS</t>
+  </si>
+  <si>
+    <t>6·PG2·PS·PT</t>
+  </si>
+  <si>
+    <t>6·PG2·PS·PC</t>
+  </si>
+  <si>
+    <t>24·PG2·PS·PT·PC</t>
+  </si>
+  <si>
+    <t>24·PG·PS·PT2·PC</t>
+  </si>
+  <si>
+    <t>24·PG·PS·PT·PC2</t>
+  </si>
+  <si>
+    <t>24·PG·PS2·PT·PC</t>
+  </si>
+  <si>
+    <t>6·PG·PS2·PT</t>
+  </si>
+  <si>
+    <t>2·PG·PS2</t>
+  </si>
+  <si>
+    <t>6·PG·PS2·PC</t>
   </si>
 </sst>
 </file>
@@ -561,6 +561,33 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -575,33 +602,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="20" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -925,93 +925,96 @@
   <dimension ref="B1:R19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J12" sqref="J12"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="6.6640625" customWidth="1"/>
+    <col min="1" max="1" width="6.6328125" customWidth="1"/>
+    <col min="6" max="8" width="13.6328125" customWidth="1"/>
+    <col min="11" max="13" width="13.6328125" customWidth="1"/>
+    <col min="16" max="18" width="13.6328125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="2" spans="2:18" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="5"/>
       <c r="C2" s="2"/>
-      <c r="D2" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
-      <c r="M2" s="22"/>
-      <c r="N2" s="22"/>
-      <c r="O2" s="22"/>
-      <c r="P2" s="22"/>
-      <c r="Q2" s="22"/>
-      <c r="R2" s="23"/>
+      <c r="D2" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E2" s="17"/>
+      <c r="F2" s="17"/>
+      <c r="G2" s="17"/>
+      <c r="H2" s="17"/>
+      <c r="I2" s="17"/>
+      <c r="J2" s="17"/>
+      <c r="K2" s="17"/>
+      <c r="L2" s="17"/>
+      <c r="M2" s="17"/>
+      <c r="N2" s="17"/>
+      <c r="O2" s="17"/>
+      <c r="P2" s="17"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="18"/>
     </row>
-    <row r="3" spans="2:18" ht="15.6" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:18" ht="15.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B3" s="6"/>
       <c r="C3" s="7"/>
-      <c r="D3" s="17">
-        <v>0</v>
-      </c>
-      <c r="E3" s="18"/>
-      <c r="F3" s="18"/>
-      <c r="G3" s="18"/>
-      <c r="H3" s="19"/>
-      <c r="I3" s="17">
-        <v>1</v>
-      </c>
-      <c r="J3" s="18"/>
-      <c r="K3" s="18"/>
-      <c r="L3" s="18"/>
-      <c r="M3" s="19"/>
-      <c r="N3" s="17">
-        <v>2</v>
-      </c>
-      <c r="O3" s="18"/>
-      <c r="P3" s="18"/>
-      <c r="Q3" s="18"/>
-      <c r="R3" s="19"/>
+      <c r="D3" s="26">
+        <v>0</v>
+      </c>
+      <c r="E3" s="27"/>
+      <c r="F3" s="27"/>
+      <c r="G3" s="27"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="26">
+        <v>1</v>
+      </c>
+      <c r="J3" s="27"/>
+      <c r="K3" s="27"/>
+      <c r="L3" s="27"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="26">
+        <v>2</v>
+      </c>
+      <c r="O3" s="27"/>
+      <c r="P3" s="27"/>
+      <c r="Q3" s="27"/>
+      <c r="R3" s="28"/>
     </row>
-    <row r="4" spans="2:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B4" s="20" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="26">
+    <row r="4" spans="2:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="21">
         <v>0</v>
       </c>
       <c r="D4" s="5"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="G4" s="15"/>
-      <c r="H4" s="16"/>
+      <c r="F4" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G4" s="24"/>
+      <c r="H4" s="25"/>
       <c r="I4" s="5"/>
       <c r="J4" s="2"/>
-      <c r="K4" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="L4" s="15"/>
-      <c r="M4" s="16"/>
+      <c r="K4" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="L4" s="24"/>
+      <c r="M4" s="25"/>
       <c r="N4" s="5"/>
       <c r="O4" s="2"/>
-      <c r="P4" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q4" s="15"/>
-      <c r="R4" s="16"/>
+      <c r="P4" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q4" s="24"/>
+      <c r="R4" s="25"/>
     </row>
-    <row r="5" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B5" s="20"/>
-      <c r="C5" s="27"/>
+    <row r="5" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B5" s="15"/>
+      <c r="C5" s="22"/>
       <c r="D5" s="6"/>
       <c r="E5" s="1"/>
       <c r="F5" s="1">
@@ -1046,10 +1049,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="6" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B6" s="20"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="24" t="s">
+    <row r="6" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B6" s="15"/>
+      <c r="C6" s="22"/>
+      <c r="D6" s="19" t="s">
         <v>3</v>
       </c>
       <c r="E6" s="1">
@@ -1064,7 +1067,7 @@
       <c r="H6" s="9" t="s">
         <v>5</v>
       </c>
-      <c r="I6" s="24" t="s">
+      <c r="I6" s="19" t="s">
         <v>3</v>
       </c>
       <c r="J6" s="1">
@@ -1074,12 +1077,12 @@
         <v>6</v>
       </c>
       <c r="L6" s="8" t="s">
-        <v>12</v>
+        <v>23</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="N6" s="24" t="s">
+        <v>40</v>
+      </c>
+      <c r="N6" s="19" t="s">
         <v>3</v>
       </c>
       <c r="O6" s="1">
@@ -1089,16 +1092,16 @@
         <v>7</v>
       </c>
       <c r="Q6" s="12" t="s">
-        <v>14</v>
+        <v>31</v>
       </c>
       <c r="R6" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B7" s="20"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="24"/>
+    <row r="7" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B7" s="15"/>
+      <c r="C7" s="22"/>
+      <c r="D7" s="19"/>
       <c r="E7" s="1">
         <v>1</v>
       </c>
@@ -1106,42 +1109,42 @@
         <v>8</v>
       </c>
       <c r="G7" s="8" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="H7" s="9" t="s">
-        <v>16</v>
-      </c>
-      <c r="I7" s="24"/>
+        <v>13</v>
+      </c>
+      <c r="I7" s="19"/>
       <c r="J7" s="1">
         <v>1</v>
       </c>
       <c r="K7" s="8" t="s">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="L7" s="8" t="s">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="N7" s="24"/>
+        <v>38</v>
+      </c>
+      <c r="N7" s="19"/>
       <c r="O7" s="1">
         <v>1</v>
       </c>
       <c r="P7" s="12" t="s">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="Q7" s="12" t="s">
-        <v>21</v>
+        <v>32</v>
       </c>
       <c r="R7" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="20"/>
-      <c r="C8" s="28"/>
-      <c r="D8" s="25"/>
+    <row r="8" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B8" s="15"/>
+      <c r="C8" s="23"/>
+      <c r="D8" s="20"/>
       <c r="E8" s="4">
         <v>2</v>
       </c>
@@ -1149,25 +1152,25 @@
         <v>9</v>
       </c>
       <c r="G8" s="10" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="H8" s="11">
         <v>0</v>
       </c>
-      <c r="I8" s="25"/>
+      <c r="I8" s="20"/>
       <c r="J8" s="4">
         <v>2</v>
       </c>
       <c r="K8" s="10" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="L8" s="10" t="s">
-        <v>23</v>
+        <v>36</v>
       </c>
       <c r="M8" s="13">
         <v>0</v>
       </c>
-      <c r="N8" s="25"/>
+      <c r="N8" s="20"/>
       <c r="O8" s="4">
         <v>2</v>
       </c>
@@ -1181,36 +1184,36 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="2:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B9" s="20"/>
-      <c r="C9" s="26">
+    <row r="9" spans="2:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B9" s="15"/>
+      <c r="C9" s="21">
         <v>1</v>
       </c>
       <c r="D9" s="5"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="G9" s="15"/>
-      <c r="H9" s="16"/>
+      <c r="F9" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G9" s="24"/>
+      <c r="H9" s="25"/>
       <c r="I9" s="5"/>
       <c r="J9" s="2"/>
-      <c r="K9" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="L9" s="15"/>
-      <c r="M9" s="16"/>
+      <c r="K9" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="L9" s="24"/>
+      <c r="M9" s="25"/>
       <c r="N9" s="5"/>
       <c r="O9" s="2"/>
-      <c r="P9" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q9" s="15"/>
-      <c r="R9" s="16"/>
+      <c r="P9" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q9" s="24"/>
+      <c r="R9" s="25"/>
     </row>
-    <row r="10" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B10" s="20"/>
-      <c r="C10" s="27"/>
+    <row r="10" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B10" s="15"/>
+      <c r="C10" s="22"/>
       <c r="D10" s="6"/>
       <c r="E10" s="1"/>
       <c r="F10" s="1">
@@ -1245,10 +1248,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B11" s="20"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="24" t="s">
+    <row r="11" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B11" s="15"/>
+      <c r="C11" s="22"/>
+      <c r="D11" s="19" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="1">
@@ -1258,158 +1261,158 @@
         <v>10</v>
       </c>
       <c r="G11" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="H11" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="I11" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="1">
+        <v>0</v>
+      </c>
+      <c r="K11" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="L11" s="8" t="s">
         <v>25</v>
       </c>
-      <c r="H11" s="9" t="s">
+      <c r="M11" s="9" t="s">
+        <v>34</v>
+      </c>
+      <c r="N11" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="O11" s="1">
+        <v>0</v>
+      </c>
+      <c r="P11" s="12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q11" s="12" t="s">
+        <v>43</v>
+      </c>
+      <c r="R11" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B12" s="15"/>
+      <c r="C12" s="22"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="1">
+        <v>1</v>
+      </c>
+      <c r="F12" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="I12" s="19"/>
+      <c r="J12" s="1">
+        <v>1</v>
+      </c>
+      <c r="K12" s="8" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="1">
-        <v>0</v>
-      </c>
-      <c r="K11" s="8" t="s">
+      <c r="L12" s="8" t="s">
+        <v>35</v>
+      </c>
+      <c r="M12" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="N12" s="19"/>
+      <c r="O12" s="1">
+        <v>1</v>
+      </c>
+      <c r="P12" s="12" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q12" s="12" t="s">
+        <v>44</v>
+      </c>
+      <c r="R12" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B13" s="15"/>
+      <c r="C13" s="23"/>
+      <c r="D13" s="20"/>
+      <c r="E13" s="4">
+        <v>2</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="G13" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="L11" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="M11" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="N11" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="O11" s="1">
-        <v>0</v>
-      </c>
-      <c r="P11" s="12" t="s">
-        <v>30</v>
-      </c>
-      <c r="Q11" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="R11" s="9">
+      <c r="H13" s="11">
+        <v>0</v>
+      </c>
+      <c r="I13" s="20"/>
+      <c r="J13" s="4">
+        <v>2</v>
+      </c>
+      <c r="K13" s="10" t="s">
+        <v>33</v>
+      </c>
+      <c r="L13" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="M13" s="11">
+        <v>0</v>
+      </c>
+      <c r="N13" s="20"/>
+      <c r="O13" s="4">
+        <v>2</v>
+      </c>
+      <c r="P13" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q13" s="10">
+        <v>0</v>
+      </c>
+      <c r="R13" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B12" s="20"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="1">
-        <v>1</v>
-      </c>
-      <c r="F12" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G12" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="H12" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="I12" s="24"/>
-      <c r="J12" s="1">
-        <v>1</v>
-      </c>
-      <c r="K12" s="8" t="s">
-        <v>37</v>
-      </c>
-      <c r="L12" s="8" t="s">
-        <v>38</v>
-      </c>
-      <c r="M12" s="9" t="s">
-        <v>39</v>
-      </c>
-      <c r="N12" s="24"/>
-      <c r="O12" s="1">
-        <v>1</v>
-      </c>
-      <c r="P12" s="12" t="s">
-        <v>40</v>
-      </c>
-      <c r="Q12" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="R12" s="9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="20"/>
-      <c r="C13" s="28"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="4">
-        <v>2</v>
-      </c>
-      <c r="F13" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="G13" s="10" t="s">
-        <v>42</v>
-      </c>
-      <c r="H13" s="11">
-        <v>0</v>
-      </c>
-      <c r="I13" s="25"/>
-      <c r="J13" s="4">
-        <v>2</v>
-      </c>
-      <c r="K13" s="10" t="s">
-        <v>43</v>
-      </c>
-      <c r="L13" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="M13" s="11">
-        <v>0</v>
-      </c>
-      <c r="N13" s="25"/>
-      <c r="O13" s="4">
-        <v>2</v>
-      </c>
-      <c r="P13" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q13" s="10">
-        <v>0</v>
-      </c>
-      <c r="R13" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="2:18" ht="15" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="20"/>
-      <c r="C14" s="26">
+    <row r="14" spans="2:18" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+      <c r="B14" s="15"/>
+      <c r="C14" s="21">
         <v>2</v>
       </c>
       <c r="D14" s="5"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="G14" s="15"/>
-      <c r="H14" s="16"/>
+      <c r="F14" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="G14" s="24"/>
+      <c r="H14" s="25"/>
       <c r="I14" s="5"/>
       <c r="J14" s="2"/>
-      <c r="K14" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="L14" s="15"/>
-      <c r="M14" s="16"/>
+      <c r="K14" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="L14" s="24"/>
+      <c r="M14" s="25"/>
       <c r="N14" s="5"/>
       <c r="O14" s="2"/>
-      <c r="P14" s="15" t="s">
-        <v>2</v>
-      </c>
-      <c r="Q14" s="15"/>
-      <c r="R14" s="16"/>
+      <c r="P14" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="Q14" s="24"/>
+      <c r="R14" s="25"/>
     </row>
-    <row r="15" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B15" s="20"/>
-      <c r="C15" s="27"/>
+    <row r="15" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B15" s="15"/>
+      <c r="C15" s="22"/>
       <c r="D15" s="6"/>
       <c r="E15" s="1"/>
       <c r="F15" s="1">
@@ -1444,10 +1447,10 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B16" s="20"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="24" t="s">
+    <row r="16" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B16" s="15"/>
+      <c r="C16" s="22"/>
+      <c r="D16" s="19" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="1">
@@ -1457,131 +1460,141 @@
         <v>11</v>
       </c>
       <c r="G16" s="8" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="H16" s="9">
         <v>0</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="I16" s="19" t="s">
         <v>3</v>
       </c>
       <c r="J16" s="1">
         <v>0</v>
       </c>
       <c r="K16" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="L16" s="8" t="s">
+        <v>50</v>
+      </c>
+      <c r="M16" s="9">
+        <v>0</v>
+      </c>
+      <c r="N16" s="19" t="s">
+        <v>3</v>
+      </c>
+      <c r="O16" s="1">
+        <v>0</v>
+      </c>
+      <c r="P16" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q16" s="8">
+        <v>0</v>
+      </c>
+      <c r="R16" s="9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="2:18" x14ac:dyDescent="0.35">
+      <c r="B17" s="15"/>
+      <c r="C17" s="22"/>
+      <c r="D17" s="19"/>
+      <c r="E17" s="1">
+        <v>1</v>
+      </c>
+      <c r="F17" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="G17" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="H17" s="9">
+        <v>0</v>
+      </c>
+      <c r="I17" s="19"/>
+      <c r="J17" s="1">
+        <v>1</v>
+      </c>
+      <c r="K17" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="L17" s="8" t="s">
         <v>47</v>
       </c>
-      <c r="L16" s="8" t="s">
-        <v>48</v>
-      </c>
-      <c r="M16" s="9">
-        <v>0</v>
-      </c>
-      <c r="N16" s="24" t="s">
-        <v>3</v>
-      </c>
-      <c r="O16" s="1">
-        <v>0</v>
-      </c>
-      <c r="P16" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q16" s="8">
-        <v>0</v>
-      </c>
-      <c r="R16" s="9">
+      <c r="M17" s="9">
+        <v>0</v>
+      </c>
+      <c r="N17" s="19"/>
+      <c r="O17" s="1">
+        <v>1</v>
+      </c>
+      <c r="P17" s="8">
+        <v>0</v>
+      </c>
+      <c r="Q17" s="8">
+        <v>0</v>
+      </c>
+      <c r="R17" s="9">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:18" x14ac:dyDescent="0.3">
-      <c r="B17" s="20"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="1">
-        <v>1</v>
-      </c>
-      <c r="F17" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="G17" s="8" t="s">
-        <v>46</v>
-      </c>
-      <c r="H17" s="9">
-        <v>0</v>
-      </c>
-      <c r="I17" s="24"/>
-      <c r="J17" s="1">
-        <v>1</v>
-      </c>
-      <c r="K17" s="8" t="s">
-        <v>49</v>
-      </c>
-      <c r="L17" s="8" t="s">
-        <v>50</v>
-      </c>
-      <c r="M17" s="9">
-        <v>0</v>
-      </c>
-      <c r="N17" s="24"/>
-      <c r="O17" s="1">
-        <v>1</v>
-      </c>
-      <c r="P17" s="8">
-        <v>0</v>
-      </c>
-      <c r="Q17" s="8">
-        <v>0</v>
-      </c>
-      <c r="R17" s="9">
+    <row r="18" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="16"/>
+      <c r="C18" s="23"/>
+      <c r="D18" s="20"/>
+      <c r="E18" s="4">
+        <v>2</v>
+      </c>
+      <c r="F18" s="10">
+        <v>0</v>
+      </c>
+      <c r="G18" s="10">
+        <v>0</v>
+      </c>
+      <c r="H18" s="11">
+        <v>0</v>
+      </c>
+      <c r="I18" s="20"/>
+      <c r="J18" s="4">
+        <v>2</v>
+      </c>
+      <c r="K18" s="10">
+        <v>0</v>
+      </c>
+      <c r="L18" s="10">
+        <v>0</v>
+      </c>
+      <c r="M18" s="14">
+        <v>0</v>
+      </c>
+      <c r="N18" s="20"/>
+      <c r="O18" s="4">
+        <v>2</v>
+      </c>
+      <c r="P18" s="10">
+        <v>0</v>
+      </c>
+      <c r="Q18" s="10">
+        <v>0</v>
+      </c>
+      <c r="R18" s="11">
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="2:18" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="21"/>
-      <c r="C18" s="28"/>
-      <c r="D18" s="25"/>
-      <c r="E18" s="4">
-        <v>2</v>
-      </c>
-      <c r="F18" s="10">
-        <v>0</v>
-      </c>
-      <c r="G18" s="10">
-        <v>0</v>
-      </c>
-      <c r="H18" s="11">
-        <v>0</v>
-      </c>
-      <c r="I18" s="25"/>
-      <c r="J18" s="4">
-        <v>2</v>
-      </c>
-      <c r="K18" s="10">
-        <v>0</v>
-      </c>
-      <c r="L18" s="10">
-        <v>0</v>
-      </c>
-      <c r="M18" s="14">
-        <v>0</v>
-      </c>
-      <c r="N18" s="25"/>
-      <c r="O18" s="4">
-        <v>2</v>
-      </c>
-      <c r="P18" s="10">
-        <v>0</v>
-      </c>
-      <c r="Q18" s="10">
-        <v>0</v>
-      </c>
-      <c r="R18" s="11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="19" spans="2:18" ht="15" thickTop="1" x14ac:dyDescent="0.3"/>
+    <row r="19" spans="2:18" ht="15" thickTop="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <mergeCells count="26">
+    <mergeCell ref="P9:R9"/>
+    <mergeCell ref="F14:H14"/>
+    <mergeCell ref="K14:M14"/>
+    <mergeCell ref="P14:R14"/>
+    <mergeCell ref="D3:H3"/>
+    <mergeCell ref="I3:M3"/>
+    <mergeCell ref="N3:R3"/>
+    <mergeCell ref="K4:M4"/>
+    <mergeCell ref="P4:R4"/>
+    <mergeCell ref="F4:H4"/>
     <mergeCell ref="B4:B18"/>
     <mergeCell ref="D2:R2"/>
     <mergeCell ref="D11:D13"/>
@@ -1598,16 +1611,6 @@
     <mergeCell ref="C14:C18"/>
     <mergeCell ref="F9:H9"/>
     <mergeCell ref="K9:M9"/>
-    <mergeCell ref="P9:R9"/>
-    <mergeCell ref="F14:H14"/>
-    <mergeCell ref="K14:M14"/>
-    <mergeCell ref="P14:R14"/>
-    <mergeCell ref="D3:H3"/>
-    <mergeCell ref="I3:M3"/>
-    <mergeCell ref="N3:R3"/>
-    <mergeCell ref="K4:M4"/>
-    <mergeCell ref="P4:R4"/>
-    <mergeCell ref="F4:H4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>